<commit_message>
Update Week 10 - Revenue Recognition.xlsx
</commit_message>
<xml_diff>
--- a/Advanced Corporate Reporting/Week 10 - Revenue Recognition.xlsx
+++ b/Advanced Corporate Reporting/Week 10 - Revenue Recognition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hudac-my.sharepoint.com/personal/u2281887_unimail_hud_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ubayd\Documents\GitHub\University-Resources\Advanced Corporate Reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="8_{234E3143-87F1-4842-8025-4513346A511E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BCFA06E-8941-4D23-BA85-6F13002A666B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B78CA4F-55E4-4952-A200-E1EE697570DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{C2469414-3BE7-4EBF-AEC1-F9E92F787D49}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11835" xr2:uid="{C2469414-3BE7-4EBF-AEC1-F9E92F787D49}"/>
   </bookViews>
   <sheets>
     <sheet name="Seminar Questions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
   <si>
     <t>Question 1:</t>
   </si>
@@ -348,6 +348,87 @@
   </si>
   <si>
     <t>treated as a sale, but shown as a cash inflow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Question 6:</t>
+  </si>
+  <si>
+    <t>Bell plc operates in the telecommunications industry. The company sells handsets to</t>
+  </si>
+  <si>
+    <t>dealers for £150 and invoices the dealers for those handsets.</t>
+  </si>
+  <si>
+    <t>The dealer can apply the handset up to a service contract being signed by a</t>
+  </si>
+  <si>
+    <t>customer.</t>
+  </si>
+  <si>
+    <t>When the customer signs the contract, the customer receives the handset free of</t>
+  </si>
+  <si>
+    <t>charge.</t>
+  </si>
+  <si>
+    <t>Bell allows the dealer a commission of £280 on the connection of a customer and the</t>
+  </si>
+  <si>
+    <t>transaction with the dealer is settled net by a payment of £130 by Bell to the dealer</t>
+  </si>
+  <si>
+    <t>being the cost of the handset to the dealer (£150) deducted from the commission</t>
+  </si>
+  <si>
+    <t>£280).</t>
+  </si>
+  <si>
+    <t>The handset cannot be sold separately by the dealer and the service contract lasts</t>
+  </si>
+  <si>
+    <t>for a 12 month period. Dealers do not sell prepaid phones and Bell receives monthly</t>
+  </si>
+  <si>
+    <t>revenue for the service contact.</t>
+  </si>
+  <si>
+    <t>The dealer may return any handsets before a service contract is signed with a</t>
+  </si>
+  <si>
+    <t>Explain, giving reasons, whether the dealer is acting as Principal or Agent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For this particular scenario, the dealer acts more as an agent than </t>
+  </si>
+  <si>
+    <t>a principal.</t>
+  </si>
+  <si>
+    <t>Firstly, the dealer does not control the pricing or sale of the handsets independently;</t>
+  </si>
+  <si>
+    <t>they are basically tied to the service contract.</t>
+  </si>
+  <si>
+    <t>The dealer's compensation is also based on a commission for each contract</t>
+  </si>
+  <si>
+    <t>signed as opposed to profit from selling goods.</t>
+  </si>
+  <si>
+    <t>The dealer can return unsold handsets, which would significantly reduce their risk</t>
+  </si>
+  <si>
+    <t>exposure, something that's more attributable to agents rather than principals.</t>
+  </si>
+  <si>
+    <t>The primary purpose is to secure customers for Bell's service contracts, with the</t>
+  </si>
+  <si>
+    <t>handsets serving as an incentive, not as the dealer's product to sell freely.</t>
   </si>
 </sst>
 </file>
@@ -358,7 +439,7 @@
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -418,21 +499,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8467E32-9C77-4BAD-92DA-584501B7C5FC}">
-  <dimension ref="B2:N78"/>
+  <dimension ref="B2:W79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="D23" zoomScale="110" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,15 +860,18 @@
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P2" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -805,8 +887,18 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -822,8 +914,18 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I5" s="3" t="s">
         <v>19</v>
       </c>
@@ -832,8 +934,16 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P5" s="3"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -843,8 +953,18 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -856,8 +976,18 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P7" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -869,8 +999,16 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P8" s="3"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -882,8 +1020,18 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I10" s="3" t="s">
         <v>22</v>
       </c>
@@ -892,8 +1040,18 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -903,8 +1061,16 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -916,8 +1082,18 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -929,8 +1105,18 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P13" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -942,8 +1128,18 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -955,16 +1151,34 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P16" s="3"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -976,8 +1190,18 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -987,8 +1211,18 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -1000,8 +1234,18 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1013,8 +1257,16 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P20" s="3"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1023,16 +1275,46 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="P22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P23" s="3"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>60</v>
       </c>
@@ -1041,8 +1323,18 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>61</v>
       </c>
@@ -1055,7 +1347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
@@ -1067,8 +1359,11 @@
       <c r="I26" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>63</v>
       </c>
@@ -1077,8 +1372,11 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1089,7 +1387,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>64</v>
       </c>
@@ -1101,8 +1399,11 @@
       <c r="I29" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>65</v>
       </c>
@@ -1114,8 +1415,11 @@
       <c r="I30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>66</v>
       </c>
@@ -1125,7 +1429,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>67</v>
       </c>
@@ -1137,8 +1441,11 @@
       <c r="I32" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>68</v>
       </c>
@@ -1150,11 +1457,14 @@
       <c r="I33" t="s">
         <v>39</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="7">
         <v>2400</v>
       </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>69</v>
       </c>
@@ -1164,7 +1474,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1174,8 +1484,11 @@
       <c r="I35" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>70</v>
       </c>
@@ -1187,8 +1500,11 @@
       <c r="I36" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>71</v>
       </c>
@@ -1198,29 +1514,32 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9" t="s">
+      <c r="J38" s="1"/>
+      <c r="K38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9" t="s">
+      <c r="L38" s="1"/>
+      <c r="M38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N38" s="9" t="s">
+      <c r="N38" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>72</v>
       </c>
@@ -1241,8 +1560,11 @@
       <c r="N39" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>73</v>
       </c>
@@ -1254,19 +1576,19 @@
       <c r="I40" t="s">
         <v>49</v>
       </c>
-      <c r="K40" s="7">
+      <c r="K40" s="5">
         <v>500</v>
       </c>
-      <c r="M40" s="8">
+      <c r="M40" s="6">
         <f>K40/K42</f>
         <v>0.19230769230769232</v>
       </c>
-      <c r="N40" s="11">
+      <c r="N40" s="8">
         <f>M33*M40</f>
         <v>461.53846153846155</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1276,19 +1598,19 @@
       <c r="I41" t="s">
         <v>50</v>
       </c>
-      <c r="K41" s="7">
+      <c r="K41" s="5">
         <v>2100</v>
       </c>
-      <c r="M41" s="8">
+      <c r="M41" s="6">
         <f>K41/K42</f>
         <v>0.80769230769230771</v>
       </c>
-      <c r="N41" s="11">
+      <c r="N41" s="8">
         <f>M33*M41</f>
         <v>1938.4615384615386</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>74</v>
       </c>
@@ -1300,19 +1622,19 @@
       <c r="I42" t="s">
         <v>51</v>
       </c>
-      <c r="K42" s="7">
+      <c r="K42" s="5">
         <v>2600</v>
       </c>
-      <c r="M42" s="8">
+      <c r="M42" s="6">
         <f>K42/K42</f>
         <v>1</v>
       </c>
-      <c r="N42" s="11">
+      <c r="N42" s="8">
         <f>M33*M42</f>
         <v>2400</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>75</v>
       </c>
@@ -1322,31 +1644,31 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="I44" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>77</v>
       </c>
       <c r="I46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="6" t="s">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>79</v>
       </c>
       <c r="I48" t="s">
@@ -1371,7 +1693,7 @@
         <v>56</v>
       </c>
       <c r="J51" s="1"/>
-      <c r="K51" s="12">
+      <c r="K51" s="9">
         <f>1938.46*(7/12)</f>
         <v>1130.7683333333334</v>
       </c>
@@ -1401,7 +1723,7 @@
       <c r="B56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I56" s="13">
+      <c r="I56" s="10">
         <f xml:space="preserve"> 1130.77+461.54</f>
         <v>1592.31</v>
       </c>
@@ -1494,6 +1816,11 @@
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1721,20 +2048,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fc68bb02-cea7-47a7-8486-5fa5775c5400" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fc68bb02-cea7-47a7-8486-5fa5775c5400" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1757,26 +2084,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E05C6A-8B1D-4D86-8A37-163F21507651}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{559E0401-8279-4456-A823-B2287B09FFE4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="fc68bb02-cea7-47a7-8486-5fa5775c5400"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="9ad45b7a-dbde-452b-a4a7-7cb6f25a272a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{559E0401-8279-4456-A823-B2287B09FFE4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E05C6A-8B1D-4D86-8A37-163F21507651}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9ad45b7a-dbde-452b-a4a7-7cb6f25a272a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fc68bb02-cea7-47a7-8486-5fa5775c5400"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>